<commit_message>
made changes in extendsReport and BaseClass.java
</commit_message>
<xml_diff>
--- a/TestData/zig.xlsx
+++ b/TestData/zig.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="37">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -729,47 +729,47 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>